<commit_message>
Update IG with latest changes including new practitioner profiles and profesiones efectores codesystem
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-BundleCabaRecupero.xlsx
+++ b/output/StructureDefinition-BundleCabaRecupero.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10059" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10059" uniqueCount="593">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-12T16:20:05-03:00</t>
+    <t>2025-07-12T17:02:17-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1497,31 +1497,31 @@
     <t>Bundle.entry:DatosEncuentro.response.outcome</t>
   </si>
   <si>
-    <t>Bundle.entry:DatosSolicitante</t>
-  </si>
-  <si>
-    <t>DatosSolicitante</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.link</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.fullUrl</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Practitioner {http://recuperocaba.gob.ar/StructureDefinition/PractitionerCabaRecupero}
+    <t>Bundle.entry:DatosProfesionalFirmante</t>
+  </si>
+  <si>
+    <t>DatosProfesionalFirmante</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.link</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.fullUrl</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practitioner {http://recuperocaba.gob.ar/StructureDefinition/PractitionerCabaFirmanteRecupero}
 </t>
   </si>
   <si>
@@ -1537,178 +1537,182 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Bundle.entry:DatosSolicitante.search</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.search.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.search.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.search.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.search.mode</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.search.score</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.method</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.url</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.ifNoneMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.ifModifiedSince</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.ifMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.request.ifNoneExist</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.status</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.location</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.etag</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.lastModified</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosSolicitante.response.outcome</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante</t>
-  </si>
-  <si>
-    <t>DatosFirmante</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.link</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.fullUrl</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.resource</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search.mode</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.search.score</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.method</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.url</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.ifNoneMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.ifModifiedSince</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.ifMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.request.ifNoneExist</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.status</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.location</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.etag</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.lastModified</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DatosFirmante.response.outcome</t>
+    <t>Bundle.entry:DatosProfesionalFirmante.search</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.search.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.search.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.search.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.search.mode</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.search.score</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.method</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.url</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.ifNoneMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.ifModifiedSince</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.ifMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.request.ifNoneExist</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.status</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.location</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.etag</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.lastModified</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalFirmante.response.outcome</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante</t>
+  </si>
+  <si>
+    <t>DatosProfesionalSolicitante</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.link</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.fullUrl</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practitioner {http://recuperocaba.gob.ar/StructureDefinition/PractitionerCabaSolicitanteRecupero}
+</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search.mode</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.search.score</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.method</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.url</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.ifNoneMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.ifModifiedSince</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.ifMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.request.ifNoneExist</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.status</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.location</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.etag</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.lastModified</t>
+  </si>
+  <si>
+    <t>Bundle.entry:DatosProfesionalSolicitante.response.outcome</t>
   </si>
   <si>
     <t>Bundle.entry:DatosAdjunto</t>
@@ -2174,9 +2178,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.3203125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="53.82421875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="32.46875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.25" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="21.75390625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="40.05078125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
@@ -27405,7 +27409,7 @@
         <v>20</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>484</v>
+        <v>522</v>
       </c>
       <c r="L223" t="s" s="2">
         <v>485</v>
@@ -27491,7 +27495,7 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B224" t="s" s="2">
         <v>251</v>
@@ -27603,7 +27607,7 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B225" t="s" s="2">
         <v>255</v>
@@ -27715,7 +27719,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B226" t="s" s="2">
         <v>256</v>
@@ -27829,7 +27833,7 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B227" t="s" s="2">
         <v>257</v>
@@ -27945,7 +27949,7 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B228" t="s" s="2">
         <v>258</v>
@@ -28059,7 +28063,7 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B229" t="s" s="2">
         <v>264</v>
@@ -28173,7 +28177,7 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B230" t="s" s="2">
         <v>269</v>
@@ -28285,7 +28289,7 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B231" t="s" s="2">
         <v>273</v>
@@ -28397,7 +28401,7 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B232" t="s" s="2">
         <v>274</v>
@@ -28511,7 +28515,7 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B233" t="s" s="2">
         <v>275</v>
@@ -28627,7 +28631,7 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B234" t="s" s="2">
         <v>276</v>
@@ -28739,7 +28743,7 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B235" t="s" s="2">
         <v>281</v>
@@ -28853,7 +28857,7 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B236" t="s" s="2">
         <v>285</v>
@@ -28965,7 +28969,7 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B237" t="s" s="2">
         <v>288</v>
@@ -29077,7 +29081,7 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B238" t="s" s="2">
         <v>290</v>
@@ -29189,7 +29193,7 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B239" t="s" s="2">
         <v>293</v>
@@ -29301,7 +29305,7 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B240" t="s" s="2">
         <v>296</v>
@@ -29413,7 +29417,7 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B241" t="s" s="2">
         <v>300</v>
@@ -29525,7 +29529,7 @@
     </row>
     <row r="242" hidden="true">
       <c r="A242" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B242" t="s" s="2">
         <v>301</v>
@@ -29639,7 +29643,7 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B243" t="s" s="2">
         <v>302</v>
@@ -29755,7 +29759,7 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B244" t="s" s="2">
         <v>303</v>
@@ -29867,7 +29871,7 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B245" t="s" s="2">
         <v>306</v>
@@ -29979,7 +29983,7 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B246" t="s" s="2">
         <v>309</v>
@@ -30093,7 +30097,7 @@
     </row>
     <row r="247" hidden="true">
       <c r="A247" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B247" t="s" s="2">
         <v>313</v>
@@ -30207,7 +30211,7 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B248" t="s" s="2">
         <v>317</v>
@@ -30321,13 +30325,13 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B249" t="s" s="2">
         <v>231</v>
       </c>
       <c r="C249" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D249" t="s" s="2">
         <v>20</v>
@@ -30435,7 +30439,7 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B250" t="s" s="2">
         <v>237</v>
@@ -30547,7 +30551,7 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B251" t="s" s="2">
         <v>238</v>
@@ -30661,7 +30665,7 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B252" t="s" s="2">
         <v>239</v>
@@ -30777,7 +30781,7 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B253" t="s" s="2">
         <v>240</v>
@@ -30889,7 +30893,7 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B254" t="s" s="2">
         <v>243</v>
@@ -31003,7 +31007,7 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B255" t="s" s="2">
         <v>247</v>
@@ -31029,16 +31033,16 @@
         <v>20</v>
       </c>
       <c r="K255" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="L255" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="M255" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="N255" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="O255" s="2"/>
       <c r="P255" t="s" s="2">
@@ -31106,10 +31110,10 @@
         <v>20</v>
       </c>
       <c r="AL255" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="AM255" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="AN255" t="s" s="2">
         <v>20</v>
@@ -31117,7 +31121,7 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B256" t="s" s="2">
         <v>251</v>
@@ -31229,7 +31233,7 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B257" t="s" s="2">
         <v>255</v>
@@ -31341,7 +31345,7 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B258" t="s" s="2">
         <v>256</v>
@@ -31455,7 +31459,7 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B259" t="s" s="2">
         <v>257</v>
@@ -31571,7 +31575,7 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B260" t="s" s="2">
         <v>258</v>
@@ -31685,7 +31689,7 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B261" t="s" s="2">
         <v>264</v>
@@ -31799,7 +31803,7 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B262" t="s" s="2">
         <v>269</v>
@@ -31911,7 +31915,7 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B263" t="s" s="2">
         <v>273</v>
@@ -32023,7 +32027,7 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B264" t="s" s="2">
         <v>274</v>
@@ -32137,7 +32141,7 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B265" t="s" s="2">
         <v>275</v>
@@ -32253,7 +32257,7 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B266" t="s" s="2">
         <v>276</v>
@@ -32365,7 +32369,7 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B267" t="s" s="2">
         <v>281</v>
@@ -32479,7 +32483,7 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B268" t="s" s="2">
         <v>285</v>
@@ -32591,7 +32595,7 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B269" t="s" s="2">
         <v>288</v>
@@ -32703,7 +32707,7 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B270" t="s" s="2">
         <v>290</v>
@@ -32815,7 +32819,7 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B271" t="s" s="2">
         <v>293</v>
@@ -32927,7 +32931,7 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B272" t="s" s="2">
         <v>296</v>
@@ -33039,7 +33043,7 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B273" t="s" s="2">
         <v>300</v>
@@ -33151,7 +33155,7 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B274" t="s" s="2">
         <v>301</v>
@@ -33265,7 +33269,7 @@
     </row>
     <row r="275" hidden="true">
       <c r="A275" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B275" t="s" s="2">
         <v>302</v>
@@ -33381,7 +33385,7 @@
     </row>
     <row r="276" hidden="true">
       <c r="A276" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B276" t="s" s="2">
         <v>303</v>
@@ -33493,7 +33497,7 @@
     </row>
     <row r="277" hidden="true">
       <c r="A277" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B277" t="s" s="2">
         <v>306</v>
@@ -33605,7 +33609,7 @@
     </row>
     <row r="278" hidden="true">
       <c r="A278" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B278" t="s" s="2">
         <v>309</v>
@@ -33719,7 +33723,7 @@
     </row>
     <row r="279" hidden="true">
       <c r="A279" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B279" t="s" s="2">
         <v>313</v>
@@ -33833,7 +33837,7 @@
     </row>
     <row r="280" hidden="true">
       <c r="A280" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B280" t="s" s="2">
         <v>317</v>
@@ -33947,10 +33951,10 @@
     </row>
     <row r="281" hidden="true">
       <c r="A281" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B281" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" t="s" s="2">
@@ -33973,19 +33977,19 @@
         <v>87</v>
       </c>
       <c r="K281" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="L281" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="M281" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="N281" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="O281" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="P281" t="s" s="2">
         <v>20</v>
@@ -34034,7 +34038,7 @@
         <v>20</v>
       </c>
       <c r="AF281" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="AG281" t="s" s="2">
         <v>77</v>

</xml_diff>